<commit_message>
Update test case with higher complexity
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khanh\Documents\GitHub\IntelligenceService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316F6975-0989-41E8-91E1-719CECF75082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F3EF8B-9083-413F-ABE8-FADE10365F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Level</t>
   </si>
@@ -81,45 +81,21 @@
     <t>Easy</t>
   </si>
   <si>
-    <t>Give me all the name of the clients</t>
-  </si>
-  <si>
-    <t>SELECT title FROM tbl_client;</t>
-  </si>
-  <si>
     <t>Basic Retrieval</t>
   </si>
   <si>
     <t xml:space="preserve">Pass </t>
   </si>
   <si>
-    <t>Find projects created after April 2024</t>
-  </si>
-  <si>
-    <t>SELECT projectDesc FROM tbl_project WHERE FromDate &gt; '2024-04-01';</t>
-  </si>
-  <si>
     <t>Conditional Retrieval</t>
   </si>
   <si>
-    <t>Find number of times the temperature is higher than 25 degree Celsius in May 2024</t>
-  </si>
-  <si>
-    <t>SELECT COUNT(*) AS 'Higher_Temperature_Count' FROM [dbo].[tbl_data] WHERE temperature &gt; 25 AND enqueuedTime_Stamp &gt;= '2024-05-01' AND enqueuedTime_Stamp &lt; '2024-06-01'</t>
-  </si>
-  <si>
     <t>Aggregation</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Find number of records captured by each device in April 2024</t>
-  </si>
-  <si>
-    <t>SELECT D.title AS 'Device Name', COUNT(*) AS 'Number of Records' FROM [dbo].[tbl_data] DA INNER JOIN dbo.tbl_devices D ON DA.device_Id = D.deviceID WHERE DA.enqueuedTime_Stamp &gt;= '2024-04-01' AND DA.enqueuedTime_Stamp &lt; '2024-05-01' GROUP BY D.title;</t>
-  </si>
-  <si>
     <t>Group By</t>
   </si>
   <si>
@@ -138,15 +114,6 @@
     <t>Predictive Analysis</t>
   </si>
   <si>
-    <t>Calculate average temperature for each device in Mar 2024</t>
-  </si>
-  <si>
-    <t>SELECT D.deviceID, AVG(D.temperature) AS 'Average Temperature' FROM [dbo].[tbl_data] D WHERE D.enqueuedTime_Stamp &gt;= '2024-03-01' AND D.enqueuedTime_Stamp &lt; '2024-04-01' GROUP BY D.deviceI</t>
-  </si>
-  <si>
-    <t>SELECT R.room AS 'Room Name', AVG(D.temperature) AS 'Average Temperature' FROM dbo.tbl_room R INNER JOIN dbo.tbl_data D ON R.id = D.roomID  GROUP BY R.room HAVING AVG(D.temperature) &gt; 25</t>
-  </si>
-  <si>
     <t>DateTime</t>
   </si>
   <si>
@@ -165,10 +132,52 @@
     <t>NA</t>
   </si>
   <si>
-    <t>which room in GlobalDWS have the highest temperature in April 2024</t>
-  </si>
-  <si>
     <t>Give me 15 days temperature forecast analysis based on historical data</t>
+  </si>
+  <si>
+    <t>What is the average, highest, and lowest temperature in globaldws in April 2024</t>
+  </si>
+  <si>
+    <t>SELECT AVG(temperature) AS 'Average Temperature', MAX(temperature) AS 'Highest Temperature', MIN(temperature) AS 'Lowest Temperature' FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-04-01' AND '2024-04-30'</t>
+  </si>
+  <si>
+    <t>How many rooms in contoso are with average temperature higher than 21 degree</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(DISTINCT room_name) AS NumberOfRooms FROM health_data_view WHERE client_name = 'Contoso' AND temperature &gt; 21 GROUP BY room_name HAVING AVG(temperature) &gt; 21</t>
+  </si>
+  <si>
+    <t>Provided that if the average temperature lower than 27 in the last 3 days, an email notification will be triggered. How many time email should be triggered in March 24 for GlobalDWS</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) AS EmailTriggers FROM (SELECT AVG(temperature) AS AvgTemperature, CAST(updated_time AS DATE) AS DateOnly FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-03-01' AND '2024-03-31' GROUP BY CAST(updated_time AS DATE) HAVING AVG(temperature) &lt; 27) AS SubQuery</t>
+  </si>
+  <si>
+    <t>In 2024, between GlobalDWS and Contoso which had higher co2 level</t>
+  </si>
+  <si>
+    <t>SELECT AVG(co2) AS Average_CO2 FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-01-01' AND '2024-12-31'; SELECT AVG(co2) AS Average_CO2 FROM health_data_view WHERE client_name = 'Contoso' AND updated_time BETWEEN '2024-01-01' AND '2024-12-31';</t>
+  </si>
+  <si>
+    <t>What is the trend of temperature in globaldws in April 2024</t>
+  </si>
+  <si>
+    <t>SELECT CAST(updated_time AS DATE) AS Date, AVG(temperature) AS AverageTemperature FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-04-01' AND '2024-04-30' GROUP BY CAST(updated_time AS DATE) ORDER BY Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Descriptive Statistics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conditional Retrieval	</t>
+  </si>
+  <si>
+    <t>Comparative Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Trend Analysis</t>
+  </si>
+  <si>
+    <t>Diagnose the cause of a significant temperature drop in Contoso in the past year.</t>
   </si>
 </sst>
 </file>
@@ -410,8 +419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F9" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F8" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F8" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Level"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Question"/>
@@ -726,18 +735,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
@@ -767,19 +776,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="82.5" customHeight="1">
@@ -787,19 +796,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="210" customHeight="1">
@@ -807,105 +816,94 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="299.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K5"/>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="165" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="69.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="43.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="208.8" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="69.75" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -934,16 +932,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
Update prompts and model for performance optimization
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khanh\Documents\GitHub\IntelligenceService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B993705D-62CA-4897-8AA5-F9975475AC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FA4FEB-FB21-4F98-805B-E0112F706BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>SELECT COUNT(*) AS EmailTriggers FROM (SELECT AVG(temperature) AS AvgTemperature, CAST(updated_time AS DATE) AS DateOnly FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-03-01' AND '2024-03-31' GROUP BY CAST(updated_time AS DATE) HAVING AVG(temperature) &lt; 27) AS SubQuery</t>
   </si>
   <si>
-    <t>In 2024, between GlobalDWS and Contoso which had higher co2 level</t>
-  </si>
-  <si>
     <t>SELECT AVG(co2) AS Average_CO2 FROM health_data_view WHERE client_name = 'GlobalDWS' AND updated_time BETWEEN '2024-01-01' AND '2024-12-31'; SELECT AVG(co2) AS Average_CO2 FROM health_data_view WHERE client_name = 'Contoso' AND updated_time BETWEEN '2024-01-01' AND '2024-12-31';</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>16s</t>
+  </si>
+  <si>
+    <t>Compare co2 level between GlobalDWS and Contoso in 2024 for the period both have data</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -797,7 +797,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="28.8">
@@ -805,13 +805,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>7</v>
@@ -820,7 +820,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="57" customHeight="1">
@@ -834,7 +834,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -843,7 +843,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="82.5" customHeight="1">
@@ -857,7 +857,7 @@
         <v>28</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -866,7 +866,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="210" customHeight="1">
@@ -889,7 +889,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="299.25" customHeight="1">
@@ -897,13 +897,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -921,13 +921,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
@@ -961,7 +961,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Update model to gpt-4o-mini
</commit_message>
<xml_diff>
--- a/test_case.xlsx
+++ b/test_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khanh\Documents\GitHub\IntelligenceService\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAF6233-E3B0-4C27-B331-674462943D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFF98C7-9428-4352-A251-4EDAF36DAA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Level</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t xml:space="preserve">Compare co2 level between GlobalDWS and Contoso in 2024 </t>
+  </si>
+  <si>
+    <t>gpt-4o-mini</t>
+  </si>
+  <si>
+    <t>16.8s</t>
   </si>
 </sst>
 </file>
@@ -459,8 +465,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H9" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:H9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:H10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Level"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Question"/>
@@ -777,10 +783,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -847,47 +853,35 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
+    <row r="3" spans="1:12" s="1" customFormat="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="5"/>
       <c r="G3" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="82.5" customHeight="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" ht="57" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>8</v>
@@ -896,50 +890,50 @@
         <v>47</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="210" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="1" customFormat="1" ht="82.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>48</v>
+      <c r="G5" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="299.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="1" customFormat="1" ht="210" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>8</v>
@@ -947,70 +941,96 @@
       <c r="G6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="1">
-        <v>12</v>
-      </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="165" customHeight="1">
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="1" customFormat="1" ht="299.25" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="3"/>
+      <c r="F7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="H7" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="69.75" customHeight="1">
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="165" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="88.8" customHeight="1">
-      <c r="A9" s="1" t="s">
+      <c r="H8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="1" customFormat="1" ht="69.75" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>38</v>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="88.8" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>